<commit_message>
add missing center soma
</commit_message>
<xml_diff>
--- a/+Soma/somaDoc_BS.xlsx
+++ b/+Soma/somaDoc_BS.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="4">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -135,18 +135,18 @@
   </sheetPr>
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C81" activeCellId="0" sqref="C81"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.2558139534884"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.0883720930233"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.7488372093023"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.2"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10697674418605"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.1209302325581"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0744186046512"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="32.6093023255814"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.5674418604651"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.35348837209302"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -337,6 +337,9 @@
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>29</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
add soma 82 and 99 to center somata
</commit_message>
<xml_diff>
--- a/+Soma/somaDoc_BS.xlsx
+++ b/+Soma/somaDoc_BS.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="4">
   <si>
     <t>id</t>
   </si>
@@ -372,8 +372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -921,6 +921,9 @@
       <c r="A83">
         <v>82</v>
       </c>
+      <c r="C83" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -1038,6 +1041,9 @@
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
+      </c>
+      <c r="C100" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>